<commit_message>
path for excel is fixed for enquiry
</commit_message>
<xml_diff>
--- a/backend/src/public/enquiries/enquiries-details.xlsx
+++ b/backend/src/public/enquiries/enquiries-details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -700,9 +700,1231 @@
         <v>45363.6733625</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>42f05dfc-ee9d-409f-8287-d476f0152dda</v>
+      </c>
+      <c r="B10" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E10" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F10" t="str">
+        <v>online</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H10" t="str">
+        <v>new</v>
+      </c>
+      <c r="I10" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J10" s="1">
+        <v>45383.49817211805</v>
+      </c>
+      <c r="K10" s="1">
+        <v>45383.49817211805</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>244ba0c4-7951-488e-8feb-81a4c53be013</v>
+      </c>
+      <c r="B11" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E11" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F11" t="str">
+        <v>online</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H11" t="str">
+        <v>new</v>
+      </c>
+      <c r="I11" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J11" s="1">
+        <v>45383.49964929398</v>
+      </c>
+      <c r="K11" s="1">
+        <v>45383.49964929398</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>b8d4c19d-8c2b-4d9e-9de4-618915360b25</v>
+      </c>
+      <c r="B12" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E12" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F12" t="str">
+        <v>online</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H12" t="str">
+        <v>new</v>
+      </c>
+      <c r="I12" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J12" s="1">
+        <v>45383.50901047454</v>
+      </c>
+      <c r="K12" s="1">
+        <v>45383.50901047454</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>5fcf8f96-0636-4f75-90cb-583d429798f7</v>
+      </c>
+      <c r="B13" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E13" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F13" t="str">
+        <v>online</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H13" t="str">
+        <v>new</v>
+      </c>
+      <c r="I13" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J13" s="1">
+        <v>45383.509776238425</v>
+      </c>
+      <c r="K13" s="1">
+        <v>45383.509776238425</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>a7b1fb7f-ca72-438b-9580-8c2ab114a660</v>
+      </c>
+      <c r="B14" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E14" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F14" t="str">
+        <v>online</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H14" t="str">
+        <v>new</v>
+      </c>
+      <c r="I14" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J14" s="1">
+        <v>45383.51035523148</v>
+      </c>
+      <c r="K14" s="1">
+        <v>45383.51035523148</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>9769dca5-8955-434d-a88a-4613c5e52c79</v>
+      </c>
+      <c r="B15" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E15" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F15" t="str">
+        <v>online</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H15" t="str">
+        <v>new</v>
+      </c>
+      <c r="I15" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J15" s="1">
+        <v>45383.51090576389</v>
+      </c>
+      <c r="K15" s="1">
+        <v>45383.51090576389</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>49d8805e-6c6e-451d-b23f-e2f26da064e7</v>
+      </c>
+      <c r="B16" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E16" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F16" t="str">
+        <v>online</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H16" t="str">
+        <v>new</v>
+      </c>
+      <c r="I16" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J16" s="1">
+        <v>45383.511081875</v>
+      </c>
+      <c r="K16" s="1">
+        <v>45383.511081875</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>bc2da9f7-6f0b-40a7-ad25-dc6367ada690</v>
+      </c>
+      <c r="B17" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E17" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F17" t="str">
+        <v>online</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H17" t="str">
+        <v>new</v>
+      </c>
+      <c r="I17" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J17" s="1">
+        <v>45383.51374568287</v>
+      </c>
+      <c r="K17" s="1">
+        <v>45383.51374568287</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>27a2555d-c763-4d5d-83af-c2b0e00d5c38</v>
+      </c>
+      <c r="B18" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E18" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F18" t="str">
+        <v>online</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H18" t="str">
+        <v>new</v>
+      </c>
+      <c r="I18" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J18" s="1">
+        <v>45383.51523292824</v>
+      </c>
+      <c r="K18" s="1">
+        <v>45383.51523292824</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>dead04ad-faf0-4712-893c-497737a02c10</v>
+      </c>
+      <c r="B19" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E19" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F19" t="str">
+        <v>online</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H19" t="str">
+        <v>new</v>
+      </c>
+      <c r="I19" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J19" s="1">
+        <v>45383.516021157404</v>
+      </c>
+      <c r="K19" s="1">
+        <v>45383.516021157404</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>dbd24adf-1fac-4a6f-9f66-74a4fe706c18</v>
+      </c>
+      <c r="B20" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E20" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F20" t="str">
+        <v>online</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H20" t="str">
+        <v>new</v>
+      </c>
+      <c r="I20" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J20" s="1">
+        <v>45383.51685658565</v>
+      </c>
+      <c r="K20" s="1">
+        <v>45383.51685658565</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>e211fd12-f674-4c46-8859-3b0980e7132b</v>
+      </c>
+      <c r="B21" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E21" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F21" t="str">
+        <v>online</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H21" t="str">
+        <v>new</v>
+      </c>
+      <c r="I21" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J21" s="1">
+        <v>45383.51784231482</v>
+      </c>
+      <c r="K21" s="1">
+        <v>45383.51784231482</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>b8dd3ee5-ef89-4c7c-9da7-0be7cb67c383</v>
+      </c>
+      <c r="B22" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E22" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F22" t="str">
+        <v>online</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H22" t="str">
+        <v>new</v>
+      </c>
+      <c r="I22" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J22" s="1">
+        <v>45383.5203053588</v>
+      </c>
+      <c r="K22" s="1">
+        <v>45383.5203053588</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>d8b0f01b-b7b4-4963-bae5-4dc8196a42d5</v>
+      </c>
+      <c r="B23" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E23" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F23" t="str">
+        <v>online</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H23" t="str">
+        <v>new</v>
+      </c>
+      <c r="I23" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J23" s="1">
+        <v>45383.58652862268</v>
+      </c>
+      <c r="K23" s="1">
+        <v>45383.58652862268</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>9812e680-aed3-46c7-a874-ab155e486928</v>
+      </c>
+      <c r="B24" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E24" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F24" t="str">
+        <v>online</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H24" t="str">
+        <v>new</v>
+      </c>
+      <c r="I24" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J24" s="1">
+        <v>45383.929316435184</v>
+      </c>
+      <c r="K24" s="1">
+        <v>45383.929316435184</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>1082c1ba-5932-4448-96f9-3329177bb361</v>
+      </c>
+      <c r="B25" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E25" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F25" t="str">
+        <v>online</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H25" t="str">
+        <v>new</v>
+      </c>
+      <c r="I25" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J25" s="1">
+        <v>45383.93091472222</v>
+      </c>
+      <c r="K25" s="1">
+        <v>45383.93091472222</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>05cf2f38-7789-4edf-815b-5af1226eb19a</v>
+      </c>
+      <c r="B26" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E26" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F26" t="str">
+        <v>online</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H26" t="str">
+        <v>new</v>
+      </c>
+      <c r="I26" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J26" s="1">
+        <v>45383.93190162037</v>
+      </c>
+      <c r="K26" s="1">
+        <v>45383.93190162037</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>f305470e-b470-4857-92d9-2028a5dc4a8c</v>
+      </c>
+      <c r="B27" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E27" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F27" t="str">
+        <v>online</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H27" t="str">
+        <v>new</v>
+      </c>
+      <c r="I27" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J27" s="1">
+        <v>45383.93999677083</v>
+      </c>
+      <c r="K27" s="1">
+        <v>45383.93999677083</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>9ce425cf-dbc2-460f-af11-1b428e0b0bbc</v>
+      </c>
+      <c r="B28" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E28" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F28" t="str">
+        <v>online</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H28" t="str">
+        <v>new</v>
+      </c>
+      <c r="I28" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J28" s="1">
+        <v>45383.94140707176</v>
+      </c>
+      <c r="K28" s="1">
+        <v>45383.94140707176</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>ad08e551-6863-4e07-b2c4-75c6a05a04fc</v>
+      </c>
+      <c r="B29" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E29" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F29" t="str">
+        <v>online</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H29" t="str">
+        <v>new</v>
+      </c>
+      <c r="I29" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J29" s="1">
+        <v>45384.37607922454</v>
+      </c>
+      <c r="K29" s="1">
+        <v>45384.37607922454</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>08f6413f-22e8-492e-936e-1c79166ac99c</v>
+      </c>
+      <c r="B30" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E30" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F30" t="str">
+        <v>online</v>
+      </c>
+      <c r="G30" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H30" t="str">
+        <v>new</v>
+      </c>
+      <c r="I30" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J30" s="1">
+        <v>45384.37788478009</v>
+      </c>
+      <c r="K30" s="1">
+        <v>45384.37788478009</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>5eb3479b-3d78-4ae0-b318-cf15fec2bdce</v>
+      </c>
+      <c r="B31" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E31" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F31" t="str">
+        <v>online</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H31" t="str">
+        <v>new</v>
+      </c>
+      <c r="I31" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J31" s="1">
+        <v>45384.41736</v>
+      </c>
+      <c r="K31" s="1">
+        <v>45384.41736</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>7cd1cd9a-485c-4327-832e-2a7c2c2944b3</v>
+      </c>
+      <c r="B32" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E32" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F32" t="str">
+        <v>online</v>
+      </c>
+      <c r="G32" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H32" t="str">
+        <v>new</v>
+      </c>
+      <c r="I32" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J32" s="1">
+        <v>45384.42468438658</v>
+      </c>
+      <c r="K32" s="1">
+        <v>45384.42468438658</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>b19ff9fc-1650-4428-a000-c6b4ee5dce6b</v>
+      </c>
+      <c r="B33" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E33" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F33" t="str">
+        <v>online</v>
+      </c>
+      <c r="G33" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H33" t="str">
+        <v>new</v>
+      </c>
+      <c r="I33" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J33" s="1">
+        <v>45384.42496109954</v>
+      </c>
+      <c r="K33" s="1">
+        <v>45384.42496109954</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>365756ac-f1e2-475a-827b-47cc2da808d1</v>
+      </c>
+      <c r="B34" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E34" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F34" t="str">
+        <v>online</v>
+      </c>
+      <c r="G34" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H34" t="str">
+        <v>new</v>
+      </c>
+      <c r="I34" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J34" s="1">
+        <v>45384.42499540509</v>
+      </c>
+      <c r="K34" s="1">
+        <v>45384.42499540509</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>f5a5b482-d777-43f4-a13d-30e83e2e23fd</v>
+      </c>
+      <c r="B35" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E35" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F35" t="str">
+        <v>online</v>
+      </c>
+      <c r="G35" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H35" t="str">
+        <v>new</v>
+      </c>
+      <c r="I35" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J35" s="1">
+        <v>45384.42858261574</v>
+      </c>
+      <c r="K35" s="1">
+        <v>45384.42858261574</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>165e818a-c955-43fd-a60c-a09de983cb33</v>
+      </c>
+      <c r="B36" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E36" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F36" t="str">
+        <v>online</v>
+      </c>
+      <c r="G36" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H36" t="str">
+        <v>new</v>
+      </c>
+      <c r="I36" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J36" s="1">
+        <v>45384.42889332176</v>
+      </c>
+      <c r="K36" s="1">
+        <v>45384.42889332176</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>e149eb31-c769-4c26-8abe-aa900771a766</v>
+      </c>
+      <c r="B37" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E37" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F37" t="str">
+        <v>online</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H37" t="str">
+        <v>new</v>
+      </c>
+      <c r="I37" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J37" s="1">
+        <v>45384.42969070602</v>
+      </c>
+      <c r="K37" s="1">
+        <v>45384.42969070602</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>aa3d87fe-42c3-46a6-bbd9-f2a701ed3af2</v>
+      </c>
+      <c r="B38" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E38" t="str">
+        <v>www.rindeumair@gmail.com</v>
+      </c>
+      <c r="F38" t="str">
+        <v>online</v>
+      </c>
+      <c r="G38" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H38" t="str">
+        <v>new</v>
+      </c>
+      <c r="I38" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J38" s="1">
+        <v>45384.432537685185</v>
+      </c>
+      <c r="K38" s="1">
+        <v>45384.432537685185</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>7a51ac9b-a6b4-45d4-b34d-0b0e9fba83ca</v>
+      </c>
+      <c r="B39" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E39" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F39" t="str">
+        <v>online</v>
+      </c>
+      <c r="G39" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H39" t="str">
+        <v>new</v>
+      </c>
+      <c r="I39" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J39" s="1">
+        <v>45384.43291740741</v>
+      </c>
+      <c r="K39" s="1">
+        <v>45384.43291740741</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>fbb42f10-f106-4fdf-90ee-8a11df91bf5e</v>
+      </c>
+      <c r="B40" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E40" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F40" t="str">
+        <v>online</v>
+      </c>
+      <c r="G40" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H40" t="str">
+        <v>new</v>
+      </c>
+      <c r="I40" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J40" s="1">
+        <v>45384.435869664354</v>
+      </c>
+      <c r="K40" s="1">
+        <v>45384.435869664354</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>054f43d6-27db-46ab-a4fc-e79d1e3e2bfa</v>
+      </c>
+      <c r="B41" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E41" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F41" t="str">
+        <v>online</v>
+      </c>
+      <c r="G41" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H41" t="str">
+        <v>new</v>
+      </c>
+      <c r="I41" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J41" s="1">
+        <v>45384.46312572917</v>
+      </c>
+      <c r="K41" s="1">
+        <v>45384.46312572917</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>0b0498f1-7fd0-4901-bbbf-86acbb6c38a9</v>
+      </c>
+      <c r="B42" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E42" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F42" t="str">
+        <v>online</v>
+      </c>
+      <c r="G42" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H42" t="str">
+        <v>new</v>
+      </c>
+      <c r="I42" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J42" s="1">
+        <v>45384.464447592596</v>
+      </c>
+      <c r="K42" s="1">
+        <v>45384.464447592596</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>74679c0d-fa62-49b6-be38-a5048ea77488</v>
+      </c>
+      <c r="B43" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Acme Corporation</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Inquiry about Product X</v>
+      </c>
+      <c r="E43" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F43" t="str">
+        <v>online</v>
+      </c>
+      <c r="G43" t="str">
+        <v>Website Contact Form</v>
+      </c>
+      <c r="H43" t="str">
+        <v>new</v>
+      </c>
+      <c r="I43" t="str">
+        <v>This is a test enquiry.</v>
+      </c>
+      <c r="J43" s="1">
+        <v>45384.464713113426</v>
+      </c>
+      <c r="K43" s="1">
+        <v>45384.464713113426</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>b8c40b73-c46f-46f4-8a85-3949ab10d32a</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Umair Rinde</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Dr.Babasaheb Ambedkar Technological University</v>
+      </c>
+      <c r="D44" t="str">
+        <v>sadsadsa</v>
+      </c>
+      <c r="E44" t="str">
+        <v>rindeusama01@gmail.com</v>
+      </c>
+      <c r="F44" t="str">
+        <v>online</v>
+      </c>
+      <c r="G44" t="str">
+        <v>for-organization</v>
+      </c>
+      <c r="H44" t="str">
+        <v>new</v>
+      </c>
+      <c r="J44" s="1">
+        <v>45384.48166884259</v>
+      </c>
+      <c r="K44" s="1">
+        <v>45384.48166884259</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L44"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update application get api
</commit_message>
<xml_diff>
--- a/backend/src/public/enquiries/enquiries-details.xlsx
+++ b/backend/src/public/enquiries/enquiries-details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -572,9 +572,105 @@
         <v>45405.71303105324</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>3a98ce58-eda0-4aa8-990c-be9e0a3131e1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Brooke Daniels</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Ochoa Merritt Inc</v>
+      </c>
+      <c r="D6" t="str">
+        <v xml:space="preserve">Nisi dolor sapiente </v>
+      </c>
+      <c r="E6" t="str">
+        <v>fyfu@mailinator.com</v>
+      </c>
+      <c r="F6" t="str">
+        <v>university</v>
+      </c>
+      <c r="G6" t="str">
+        <v>for-organization</v>
+      </c>
+      <c r="H6" t="str">
+        <v>new</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45434.77850829861</v>
+      </c>
+      <c r="K6" s="1">
+        <v>45434.77850829861</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2139c963-0efb-4ecf-8f66-28129184f8ed</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Umair Rinde</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Clarke and Castro Trading</v>
+      </c>
+      <c r="D7" t="str">
+        <v xml:space="preserve">Officiis voluptates </v>
+      </c>
+      <c r="E7" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F7" t="str">
+        <v>online</v>
+      </c>
+      <c r="G7" t="str">
+        <v>for-organization</v>
+      </c>
+      <c r="H7" t="str">
+        <v>new</v>
+      </c>
+      <c r="J7" s="1">
+        <v>45434.77882318287</v>
+      </c>
+      <c r="K7" s="1">
+        <v>45434.77882318287</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>c226674c-7f3c-436a-ae2b-f3f7391b952b</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Umair Rinde</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Goff Walsh Plc</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Officia eligendi dic</v>
+      </c>
+      <c r="E8" t="str">
+        <v>rindeumair@gmail.com</v>
+      </c>
+      <c r="F8" t="str">
+        <v>online</v>
+      </c>
+      <c r="G8" t="str">
+        <v>for-partnership</v>
+      </c>
+      <c r="H8" t="str">
+        <v>new</v>
+      </c>
+      <c r="J8" s="1">
+        <v>45434.77936392361</v>
+      </c>
+      <c r="K8" s="1">
+        <v>45434.77936392361</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>